<commit_message>
corrected values in table
</commit_message>
<xml_diff>
--- a/SupplementaryTables/TechnoEconomicInclusionDatasets.xlsx
+++ b/SupplementaryTables/TechnoEconomicInclusionDatasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\ASSET\supplyCurve\analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\ASSET_Development\SupplementaryTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DC78B1A-C86B-447C-BDEC-FCF709A45EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD85590-A43B-4B19-91C3-BBF12AD34116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7995" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D5F25A27-0875-4632-B875-24916052A9CA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Technology</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Rivers</t>
   </si>
   <si>
-    <t>1000m buffer (Solar); 5000m buffer (Wind)</t>
-  </si>
-  <si>
     <t>Included</t>
   </si>
   <si>
@@ -102,6 +99,18 @@
   </si>
   <si>
     <t>Argonne Natonal Lab Energy Zones Mapping Tool</t>
+  </si>
+  <si>
+    <t>250m Buffer</t>
+  </si>
+  <si>
+    <t>1000m Buffer</t>
+  </si>
+  <si>
+    <t>500m Buffer (Solar); 1000m Buffer (Wind)</t>
+  </si>
+  <si>
+    <t>1000m Buffer (Solar); 5000m Buffer (Wind)</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,138 +499,138 @@
     </row>
     <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>